<commit_message>
Updated burndown + Retrospective
</commit_message>
<xml_diff>
--- a/Assignment Files/Burndown Charts.xlsx
+++ b/Assignment Files/Burndown Charts.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop Back\Django\musicschool\Assignment Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johns\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6690E839-4062-40C8-8F00-827B2444F92D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{15417CC1-770B-4B50-8AF0-7426D5932CA7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 &amp; 2 Burndown" sheetId="1" r:id="rId1"/>
     <sheet name="Release Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Actual</t>
   </si>
@@ -108,11 +107,14 @@
   <si>
     <t>1. At around 17 days, we were ahead of schedule</t>
   </si>
+  <si>
+    <t>* less removed stories</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,18 +228,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -249,6 +239,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -861,6 +863,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -868,7 +871,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1427,6 +1429,7 @@
         <c:axId val="550969968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1580,6 +1583,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1587,7 +1591,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1767,7 +1770,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>141</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>47</c:v>
@@ -1828,10 +1831,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>141</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2121,6 +2124,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2128,7 +2132,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4245,28 +4248,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C03FC7E-C1AE-4AE9-B691-62CDE33704DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -4280,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>43187</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>43188</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>43189</v>
       </c>
@@ -4336,7 +4339,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>43190</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>43191</v>
       </c>
@@ -4364,7 +4367,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>43192</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>43193</v>
       </c>
@@ -4392,7 +4395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>43194</v>
       </c>
@@ -4409,7 +4412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>43205</v>
       </c>
@@ -4426,7 +4429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>43206</v>
       </c>
@@ -4440,7 +4443,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>43207</v>
       </c>
@@ -4454,7 +4457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>43208</v>
       </c>
@@ -4468,7 +4471,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>43209</v>
       </c>
@@ -4482,7 +4485,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>43210</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>43211</v>
       </c>
@@ -4510,7 +4513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>43212</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>43213</v>
       </c>
@@ -4538,7 +4541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>43214</v>
       </c>
@@ -4552,7 +4555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>43215</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="4">
         <v>43216</v>
       </c>
@@ -4583,7 +4586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="4">
         <v>43217</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="4">
         <v>43218</v>
       </c>
@@ -4617,7 +4620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="4">
         <v>43219</v>
       </c>
@@ -4634,7 +4637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>43220</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>43221</v>
       </c>
@@ -4662,7 +4665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>43222</v>
       </c>
@@ -4676,35 +4679,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A32" s="9"/>
     </row>
-    <row r="33" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:29" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
       <c r="Y34" s="8"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-    </row>
-    <row r="35" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z34" s="20"/>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="20"/>
+    </row>
+    <row r="35" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
@@ -4717,17 +4720,17 @@
       <c r="D35" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="U35" s="18"/>
-      <c r="V35" s="18"/>
-      <c r="W35" s="18"/>
-      <c r="X35" s="18"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
       <c r="Y35" s="8"/>
-      <c r="Z35" s="18"/>
-      <c r="AA35" s="18"/>
-      <c r="AB35" s="18"/>
-      <c r="AC35" s="18"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+      <c r="AB35" s="14"/>
+      <c r="AC35" s="14"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4741,16 +4744,16 @@
         <v>50</v>
       </c>
       <c r="U36" s="8"/>
-      <c r="V36" s="19"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
-      <c r="AA36" s="19"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="19"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>43222</v>
       </c>
@@ -4763,17 +4766,17 @@
       <c r="D37" s="3">
         <v>50</v>
       </c>
-      <c r="U37" s="20"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
       <c r="Y37" s="8"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>43223</v>
       </c>
@@ -4786,17 +4789,17 @@
       <c r="D38" s="3">
         <v>50</v>
       </c>
-      <c r="U38" s="20"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
       <c r="Y38" s="8"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>43224</v>
       </c>
@@ -4809,17 +4812,17 @@
       <c r="D39" s="3">
         <v>50</v>
       </c>
-      <c r="U39" s="20"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
       <c r="Y39" s="8"/>
-      <c r="Z39" s="20"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>43225</v>
       </c>
@@ -4832,17 +4835,17 @@
       <c r="D40" s="3">
         <v>50</v>
       </c>
-      <c r="U40" s="20"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
       <c r="Y40" s="8"/>
-      <c r="Z40" s="20"/>
-      <c r="AA40" s="19"/>
-      <c r="AB40" s="19"/>
-      <c r="AC40" s="19"/>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z40" s="16"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>43226</v>
       </c>
@@ -4855,17 +4858,17 @@
       <c r="D41" s="3">
         <v>50</v>
       </c>
-      <c r="U41" s="20"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
       <c r="Y41" s="8"/>
-      <c r="Z41" s="20"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="19"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>43227</v>
       </c>
@@ -4878,17 +4881,17 @@
       <c r="D42" s="3">
         <v>50</v>
       </c>
-      <c r="U42" s="20"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
       <c r="Y42" s="8"/>
-      <c r="Z42" s="20"/>
-      <c r="AA42" s="19"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="19"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z42" s="16"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>43228</v>
       </c>
@@ -4901,17 +4904,17 @@
       <c r="D43" s="3">
         <v>50</v>
       </c>
-      <c r="U43" s="20"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
       <c r="Y43" s="8"/>
-      <c r="Z43" s="20"/>
-      <c r="AA43" s="19"/>
-      <c r="AB43" s="19"/>
-      <c r="AC43" s="19"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>43229</v>
       </c>
@@ -4924,17 +4927,17 @@
       <c r="D44" s="3">
         <v>35</v>
       </c>
-      <c r="U44" s="20"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="21"/>
-      <c r="X44" s="19"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="15"/>
       <c r="Y44" s="8"/>
-      <c r="Z44" s="20"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="19"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>43230</v>
       </c>
@@ -4947,17 +4950,17 @@
       <c r="D45" s="3">
         <v>35</v>
       </c>
-      <c r="U45" s="20"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="21"/>
-      <c r="X45" s="19"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="15"/>
       <c r="Y45" s="8"/>
-      <c r="Z45" s="20"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>43231</v>
       </c>
@@ -4970,17 +4973,17 @@
       <c r="D46" s="3">
         <v>35</v>
       </c>
-      <c r="U46" s="20"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="19"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="15"/>
       <c r="Y46" s="8"/>
-      <c r="Z46" s="20"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="15"/>
+      <c r="AB46" s="15"/>
+      <c r="AC46" s="15"/>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>43232</v>
       </c>
@@ -4993,17 +4996,17 @@
       <c r="D47" s="3">
         <v>35</v>
       </c>
-      <c r="U47" s="20"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="21"/>
-      <c r="X47" s="19"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="15"/>
       <c r="Y47" s="8"/>
-      <c r="Z47" s="20"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="19"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>43233</v>
       </c>
@@ -5016,17 +5019,17 @@
       <c r="D48" s="3">
         <v>35</v>
       </c>
-      <c r="U48" s="20"/>
-      <c r="V48" s="19"/>
-      <c r="W48" s="21"/>
-      <c r="X48" s="19"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="15"/>
       <c r="Y48" s="8"/>
-      <c r="Z48" s="20"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="19"/>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="15"/>
+      <c r="AC48" s="15"/>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>43234</v>
       </c>
@@ -5039,17 +5042,17 @@
       <c r="D49" s="3">
         <v>35</v>
       </c>
-      <c r="U49" s="20"/>
-      <c r="V49" s="19"/>
-      <c r="W49" s="21"/>
-      <c r="X49" s="19"/>
+      <c r="U49" s="16"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="15"/>
       <c r="Y49" s="8"/>
-      <c r="Z49" s="20"/>
-      <c r="AA49" s="19"/>
-      <c r="AB49" s="19"/>
-      <c r="AC49" s="19"/>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="15"/>
+      <c r="AB49" s="15"/>
+      <c r="AC49" s="15"/>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>43235</v>
       </c>
@@ -5062,17 +5065,17 @@
       <c r="D50" s="3">
         <v>35</v>
       </c>
-      <c r="U50" s="20"/>
-      <c r="V50" s="19"/>
-      <c r="W50" s="19"/>
-      <c r="X50" s="19"/>
+      <c r="U50" s="16"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
       <c r="Y50" s="8"/>
-      <c r="Z50" s="20"/>
-      <c r="AA50" s="19"/>
-      <c r="AB50" s="19"/>
-      <c r="AC50" s="19"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="15"/>
+      <c r="AB50" s="15"/>
+      <c r="AC50" s="15"/>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
         <v>43236</v>
       </c>
@@ -5085,17 +5088,17 @@
       <c r="D51" s="3">
         <v>20</v>
       </c>
-      <c r="U51" s="20"/>
-      <c r="V51" s="19"/>
-      <c r="W51" s="19"/>
-      <c r="X51" s="19"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
       <c r="Y51" s="8"/>
-      <c r="Z51" s="20"/>
-      <c r="AA51" s="19"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="19"/>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="15"/>
+      <c r="AC51" s="15"/>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A52" s="4">
         <v>43237</v>
       </c>
@@ -5108,17 +5111,17 @@
       <c r="D52" s="3">
         <v>20</v>
       </c>
-      <c r="U52" s="20"/>
-      <c r="V52" s="19"/>
-      <c r="W52" s="19"/>
-      <c r="X52" s="19"/>
+      <c r="U52" s="16"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="15"/>
       <c r="Y52" s="8"/>
-      <c r="Z52" s="20"/>
-      <c r="AA52" s="19"/>
-      <c r="AB52" s="19"/>
-      <c r="AC52" s="19"/>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="15"/>
+      <c r="AB52" s="15"/>
+      <c r="AC52" s="15"/>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A53" s="4">
         <v>43238</v>
       </c>
@@ -5131,17 +5134,17 @@
       <c r="D53" s="3">
         <v>20</v>
       </c>
-      <c r="U53" s="20"/>
-      <c r="V53" s="19"/>
-      <c r="W53" s="19"/>
-      <c r="X53" s="19"/>
+      <c r="U53" s="16"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
       <c r="Y53" s="8"/>
-      <c r="Z53" s="20"/>
-      <c r="AA53" s="19"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="19"/>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="15"/>
+      <c r="AB53" s="15"/>
+      <c r="AC53" s="15"/>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
         <v>43239</v>
       </c>
@@ -5154,17 +5157,17 @@
       <c r="D54" s="3">
         <v>20</v>
       </c>
-      <c r="U54" s="20"/>
-      <c r="V54" s="19"/>
-      <c r="W54" s="19"/>
-      <c r="X54" s="19"/>
+      <c r="U54" s="16"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
       <c r="Y54" s="8"/>
-      <c r="Z54" s="20"/>
-      <c r="AA54" s="19"/>
-      <c r="AB54" s="19"/>
-      <c r="AC54" s="19"/>
-    </row>
-    <row r="55" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="15"/>
+      <c r="AB54" s="15"/>
+      <c r="AC54" s="15"/>
+    </row>
+    <row r="55" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A55" s="4">
         <v>43240</v>
       </c>
@@ -5180,17 +5183,17 @@
       <c r="G55" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="U55" s="20"/>
-      <c r="V55" s="19"/>
-      <c r="W55" s="19"/>
-      <c r="X55" s="19"/>
+      <c r="U55" s="16"/>
+      <c r="V55" s="15"/>
+      <c r="W55" s="15"/>
+      <c r="X55" s="15"/>
       <c r="Y55" s="8"/>
-      <c r="Z55" s="20"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="19"/>
-    </row>
-    <row r="56" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="15"/>
+      <c r="AB55" s="15"/>
+      <c r="AC55" s="15"/>
+    </row>
+    <row r="56" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="4">
         <v>43241</v>
       </c>
@@ -5206,17 +5209,17 @@
       <c r="G56" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="U56" s="20"/>
-      <c r="V56" s="19"/>
-      <c r="W56" s="19"/>
-      <c r="X56" s="19"/>
+      <c r="U56" s="16"/>
+      <c r="V56" s="15"/>
+      <c r="W56" s="15"/>
+      <c r="X56" s="15"/>
       <c r="Y56" s="8"/>
-      <c r="Z56" s="20"/>
-      <c r="AA56" s="19"/>
-      <c r="AB56" s="19"/>
-      <c r="AC56" s="19"/>
-    </row>
-    <row r="57" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z56" s="16"/>
+      <c r="AA56" s="15"/>
+      <c r="AB56" s="15"/>
+      <c r="AC56" s="15"/>
+    </row>
+    <row r="57" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A57" s="4">
         <v>43242</v>
       </c>
@@ -5232,17 +5235,17 @@
       <c r="G57" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="U57" s="20"/>
-      <c r="V57" s="19"/>
-      <c r="W57" s="19"/>
-      <c r="X57" s="19"/>
+      <c r="U57" s="16"/>
+      <c r="V57" s="15"/>
+      <c r="W57" s="15"/>
+      <c r="X57" s="15"/>
       <c r="Y57" s="8"/>
-      <c r="Z57" s="20"/>
-      <c r="AA57" s="19"/>
-      <c r="AB57" s="19"/>
-      <c r="AC57" s="19"/>
-    </row>
-    <row r="58" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z57" s="16"/>
+      <c r="AA57" s="15"/>
+      <c r="AB57" s="15"/>
+      <c r="AC57" s="15"/>
+    </row>
+    <row r="58" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="4">
         <v>43243</v>
       </c>
@@ -5258,17 +5261,17 @@
       <c r="G58" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="U58" s="20"/>
-      <c r="V58" s="19"/>
-      <c r="W58" s="19"/>
-      <c r="X58" s="19"/>
+      <c r="U58" s="16"/>
+      <c r="V58" s="15"/>
+      <c r="W58" s="15"/>
+      <c r="X58" s="15"/>
       <c r="Y58" s="8"/>
-      <c r="Z58" s="20"/>
-      <c r="AA58" s="19"/>
-      <c r="AB58" s="19"/>
-      <c r="AC58" s="19"/>
-    </row>
-    <row r="59" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z58" s="16"/>
+      <c r="AA58" s="15"/>
+      <c r="AB58" s="15"/>
+      <c r="AC58" s="15"/>
+    </row>
+    <row r="59" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="4">
         <v>43244</v>
       </c>
@@ -5284,17 +5287,17 @@
       <c r="G59" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="U59" s="20"/>
-      <c r="V59" s="19"/>
-      <c r="W59" s="19"/>
-      <c r="X59" s="19"/>
+      <c r="U59" s="16"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="15"/>
+      <c r="X59" s="15"/>
       <c r="Y59" s="8"/>
-      <c r="Z59" s="20"/>
-      <c r="AA59" s="19"/>
-      <c r="AB59" s="19"/>
-      <c r="AC59" s="19"/>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z59" s="16"/>
+      <c r="AA59" s="15"/>
+      <c r="AB59" s="15"/>
+      <c r="AC59" s="15"/>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A60" s="4">
         <v>43245</v>
       </c>
@@ -5307,17 +5310,17 @@
       <c r="D60" s="3">
         <v>5</v>
       </c>
-      <c r="U60" s="20"/>
-      <c r="V60" s="19"/>
-      <c r="W60" s="19"/>
-      <c r="X60" s="19"/>
+      <c r="U60" s="16"/>
+      <c r="V60" s="15"/>
+      <c r="W60" s="15"/>
+      <c r="X60" s="15"/>
       <c r="Y60" s="8"/>
-      <c r="Z60" s="20"/>
-      <c r="AA60" s="19"/>
-      <c r="AB60" s="19"/>
-      <c r="AC60" s="19"/>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z60" s="16"/>
+      <c r="AA60" s="15"/>
+      <c r="AB60" s="15"/>
+      <c r="AC60" s="15"/>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A61" s="4">
         <v>43246</v>
       </c>
@@ -5330,17 +5333,17 @@
       <c r="D61" s="3">
         <v>5</v>
       </c>
-      <c r="U61" s="20"/>
-      <c r="V61" s="19"/>
-      <c r="W61" s="19"/>
-      <c r="X61" s="19"/>
+      <c r="U61" s="16"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="15"/>
+      <c r="X61" s="15"/>
       <c r="Y61" s="8"/>
-      <c r="Z61" s="20"/>
-      <c r="AA61" s="19"/>
-      <c r="AB61" s="19"/>
-      <c r="AC61" s="19"/>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z61" s="16"/>
+      <c r="AA61" s="15"/>
+      <c r="AB61" s="15"/>
+      <c r="AC61" s="15"/>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A62" s="4">
         <v>43247</v>
       </c>
@@ -5353,17 +5356,17 @@
       <c r="D62" s="3">
         <v>5</v>
       </c>
-      <c r="U62" s="20"/>
-      <c r="V62" s="19"/>
-      <c r="W62" s="19"/>
-      <c r="X62" s="19"/>
+      <c r="U62" s="16"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="15"/>
+      <c r="X62" s="15"/>
       <c r="Y62" s="8"/>
-      <c r="Z62" s="20"/>
-      <c r="AA62" s="19"/>
-      <c r="AB62" s="19"/>
-      <c r="AC62" s="19"/>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z62" s="16"/>
+      <c r="AA62" s="15"/>
+      <c r="AB62" s="15"/>
+      <c r="AC62" s="15"/>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A63" s="4">
         <v>43248</v>
       </c>
@@ -5376,17 +5379,17 @@
       <c r="D63" s="3">
         <v>5</v>
       </c>
-      <c r="U63" s="20"/>
-      <c r="V63" s="22"/>
-      <c r="W63" s="19"/>
-      <c r="X63" s="19"/>
+      <c r="U63" s="16"/>
+      <c r="V63" s="18"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
       <c r="Y63" s="8"/>
-      <c r="Z63" s="20"/>
-      <c r="AA63" s="22"/>
-      <c r="AB63" s="19"/>
-      <c r="AC63" s="19"/>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z63" s="16"/>
+      <c r="AA63" s="18"/>
+      <c r="AB63" s="15"/>
+      <c r="AC63" s="15"/>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A64" s="4">
         <v>43249</v>
       </c>
@@ -5399,17 +5402,17 @@
       <c r="D64" s="3">
         <v>5</v>
       </c>
-      <c r="U64" s="20"/>
-      <c r="V64" s="22"/>
-      <c r="W64" s="19"/>
-      <c r="X64" s="19"/>
+      <c r="U64" s="16"/>
+      <c r="V64" s="18"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
       <c r="Y64" s="8"/>
-      <c r="Z64" s="20"/>
-      <c r="AA64" s="22"/>
-      <c r="AB64" s="19"/>
-      <c r="AC64" s="19"/>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z64" s="16"/>
+      <c r="AA64" s="18"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A65" s="4">
         <v>43250</v>
       </c>
@@ -5422,28 +5425,28 @@
       <c r="D65" s="1">
         <v>0</v>
       </c>
-      <c r="U65" s="20"/>
-      <c r="V65" s="22"/>
-      <c r="W65" s="19"/>
+      <c r="U65" s="16"/>
+      <c r="V65" s="18"/>
+      <c r="W65" s="15"/>
       <c r="X65" s="8"/>
       <c r="Y65" s="8"/>
-      <c r="Z65" s="20"/>
-      <c r="AA65" s="22"/>
-      <c r="AB65" s="19"/>
+      <c r="Z65" s="16"/>
+      <c r="AA65" s="18"/>
+      <c r="AB65" s="15"/>
       <c r="AC65" s="8"/>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
@@ -5462,28 +5465,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A555D3-F939-4FAE-A8B2-B32231AE9574}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.1328125" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -5494,18 +5497,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="3">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="C3" s="3">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>137+50</f>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -5513,10 +5517,10 @@
         <v>47</v>
       </c>
       <c r="C4" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -5527,22 +5531,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="12" t="s">
         <v>18</v>
       </c>

</xml_diff>